<commit_message>
Update sorting DDT test cases
</commit_message>
<xml_diff>
--- a/Test Case_Sauce Demo.xlsx
+++ b/Test Case_Sauce Demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Katalon Studio\sauceDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897E6DD3-BD80-4467-BBEC-8E7CA0501DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CC0AD2-C8E4-4613-87BD-2446B30D4618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1017,33 +1017,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1092,14 +1065,38 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1107,11 +1104,14 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1705,16 +1705,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="33" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="35"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -1726,16 +1726,16 @@
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="36">
+      <c r="B2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="27">
         <v>46113</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="35"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="26"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1747,16 +1747,16 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="31"/>
-      <c r="F3" s="32"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="23"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -1768,11 +1768,11 @@
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
@@ -1793,9 +1793,9 @@
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
       <c r="D5" s="11">
         <v>0</v>
       </c>
@@ -1897,121 +1897,121 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="A9" s="31">
         <v>1</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="I9" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="L9" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12" t="s">
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
     </row>
     <row r="13" spans="1:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
     </row>
     <row r="14" spans="1:15" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>2</v>
       </c>
-      <c r="B14" s="16"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="8" t="s">
         <v>60</v>
       </c>
@@ -2049,102 +2049,102 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15">
+      <c r="A15" s="31">
         <v>3</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="12" t="s">
+      <c r="B15" s="32"/>
+      <c r="C15" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="18" t="s">
+      <c r="I15" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="J15" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="K15" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="L15" s="12" t="s">
+      <c r="L15" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="18" t="s">
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="34" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="19"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="35"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="19"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="35"/>
     </row>
     <row r="18" spans="1:15" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="20"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="36"/>
     </row>
     <row r="19" spans="1:15" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>4</v>
       </c>
-      <c r="B19" s="16"/>
+      <c r="B19" s="32"/>
       <c r="C19" s="8" t="s">
         <v>60</v>
       </c>
@@ -2185,7 +2185,7 @@
       <c r="A20" s="7">
         <v>5</v>
       </c>
-      <c r="B20" s="16"/>
+      <c r="B20" s="32"/>
       <c r="C20" s="8" t="s">
         <v>60</v>
       </c>
@@ -2226,7 +2226,7 @@
       <c r="A21" s="7">
         <v>6</v>
       </c>
-      <c r="B21" s="16"/>
+      <c r="B21" s="32"/>
       <c r="C21" s="8" t="s">
         <v>60</v>
       </c>
@@ -2267,7 +2267,7 @@
       <c r="A22" s="7">
         <v>7</v>
       </c>
-      <c r="B22" s="16"/>
+      <c r="B22" s="32"/>
       <c r="C22" s="8" t="s">
         <v>60</v>
       </c>
@@ -2308,7 +2308,7 @@
       <c r="A23" s="7">
         <v>8</v>
       </c>
-      <c r="B23" s="16"/>
+      <c r="B23" s="32"/>
       <c r="C23" s="8" t="s">
         <v>60</v>
       </c>
@@ -2349,7 +2349,7 @@
       <c r="A24" s="7">
         <v>9</v>
       </c>
-      <c r="B24" s="16"/>
+      <c r="B24" s="32"/>
       <c r="C24" s="8" t="s">
         <v>60</v>
       </c>
@@ -2390,7 +2390,7 @@
       <c r="A25" s="7">
         <v>10</v>
       </c>
-      <c r="B25" s="16"/>
+      <c r="B25" s="32"/>
       <c r="C25" s="8" t="s">
         <v>60</v>
       </c>
@@ -2431,7 +2431,7 @@
       <c r="A26" s="7">
         <v>11</v>
       </c>
-      <c r="B26" s="16"/>
+      <c r="B26" s="32"/>
       <c r="C26" s="8" t="s">
         <v>60</v>
       </c>
@@ -2472,7 +2472,7 @@
       <c r="A27" s="7">
         <v>12</v>
       </c>
-      <c r="B27" s="16"/>
+      <c r="B27" s="32"/>
       <c r="C27" s="8" t="s">
         <v>60</v>
       </c>
@@ -2510,102 +2510,102 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
+      <c r="A28" s="31">
         <v>13</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="12" t="s">
+      <c r="B28" s="32"/>
+      <c r="C28" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="E28" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="18" t="s">
+      <c r="G28" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="H28" s="18" t="s">
+      <c r="H28" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="I28" s="18" t="s">
+      <c r="I28" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="J28" s="12" t="s">
+      <c r="J28" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="K28" s="12" t="s">
+      <c r="K28" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="L28" s="12" t="s">
+      <c r="L28" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="18" t="s">
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="34" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="19"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
+      <c r="O29" s="35"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="19"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="29"/>
+      <c r="O30" s="35"/>
     </row>
     <row r="31" spans="1:15" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-      <c r="N31" s="14"/>
-      <c r="O31" s="20"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="36"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="30"/>
+      <c r="L31" s="30"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="30"/>
+      <c r="O31" s="36"/>
     </row>
     <row r="32" spans="1:15" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>14</v>
       </c>
-      <c r="B32" s="16"/>
+      <c r="B32" s="32"/>
       <c r="C32" s="8" t="s">
         <v>51</v>
       </c>
@@ -2646,7 +2646,7 @@
       <c r="A33" s="7">
         <v>15</v>
       </c>
-      <c r="B33" s="16"/>
+      <c r="B33" s="32"/>
       <c r="C33" s="8" t="s">
         <v>51</v>
       </c>
@@ -2688,7 +2688,7 @@
         <f>SUM(A33+1)</f>
         <v>16</v>
       </c>
-      <c r="B34" s="16"/>
+      <c r="B34" s="32"/>
       <c r="C34" s="8" t="s">
         <v>51</v>
       </c>
@@ -2730,7 +2730,7 @@
         <f t="shared" ref="A35:A36" si="0">SUM(A34+1)</f>
         <v>17</v>
       </c>
-      <c r="B35" s="16"/>
+      <c r="B35" s="32"/>
       <c r="C35" s="8" t="s">
         <v>51</v>
       </c>
@@ -2772,7 +2772,7 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B36" s="17"/>
+      <c r="B36" s="33"/>
       <c r="C36" s="8" t="s">
         <v>51</v>
       </c>
@@ -2811,13 +2811,33 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="A4:C5"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="D9:D13"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="B9:B36"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="E9:E13"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="I28:I31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="H9:H13"/>
+    <mergeCell ref="I9:I13"/>
+    <mergeCell ref="I15:I18"/>
+    <mergeCell ref="H15:H18"/>
+    <mergeCell ref="G28:G31"/>
+    <mergeCell ref="O28:O31"/>
+    <mergeCell ref="L15:L18"/>
+    <mergeCell ref="M15:M18"/>
+    <mergeCell ref="N15:N18"/>
+    <mergeCell ref="O15:O18"/>
+    <mergeCell ref="J28:J31"/>
+    <mergeCell ref="K28:K31"/>
+    <mergeCell ref="L28:L31"/>
+    <mergeCell ref="M28:M31"/>
+    <mergeCell ref="N28:N31"/>
     <mergeCell ref="N9:N13"/>
     <mergeCell ref="O9:O13"/>
     <mergeCell ref="A15:A18"/>
@@ -2834,33 +2854,13 @@
     <mergeCell ref="K9:K13"/>
     <mergeCell ref="L9:L13"/>
     <mergeCell ref="M9:M13"/>
-    <mergeCell ref="J28:J31"/>
-    <mergeCell ref="K28:K31"/>
-    <mergeCell ref="L28:L31"/>
-    <mergeCell ref="M28:M31"/>
-    <mergeCell ref="N28:N31"/>
-    <mergeCell ref="O28:O31"/>
-    <mergeCell ref="L15:L18"/>
-    <mergeCell ref="M15:M18"/>
-    <mergeCell ref="N15:N18"/>
-    <mergeCell ref="O15:O18"/>
-    <mergeCell ref="E9:E13"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="I28:I31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="F28:F31"/>
-    <mergeCell ref="H9:H13"/>
-    <mergeCell ref="I9:I13"/>
-    <mergeCell ref="I15:I18"/>
-    <mergeCell ref="H15:H18"/>
-    <mergeCell ref="G28:G31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="D9:D13"/>
-    <mergeCell ref="C9:C13"/>
-    <mergeCell ref="B9:B36"/>
-    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A4:C5"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="G19:I28 G32:I36">
@@ -2964,7 +2964,7 @@
     <sheetView tabSelected="1" topLeftCell="A8" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A8" sqref="A8"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2987,16 +2987,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="33" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="35"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -3008,16 +3008,16 @@
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="36">
+      <c r="B2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="27">
         <v>46113</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="43"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="38"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -3029,16 +3029,16 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="40"/>
-      <c r="F3" s="41"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -3050,11 +3050,11 @@
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
@@ -3075,9 +3075,9 @@
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
       <c r="D5" s="11">
         <v>0</v>
       </c>
@@ -3179,122 +3179,122 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="37">
+      <c r="A9" s="41">
         <v>1</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="F9" s="39" t="s">
+      <c r="F9" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="I9" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="J9" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="L9" s="12" t="s">
+      <c r="L9" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12" t="s">
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
     </row>
     <row r="14" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>2</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
       <c r="D14" s="8" t="s">
         <v>155</v>
       </c>
@@ -3329,103 +3329,103 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="37">
+      <c r="A15" s="41">
         <v>3</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="39" t="s">
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="F15" s="39" t="s">
+      <c r="F15" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="18" t="s">
+      <c r="I15" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="J15" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="K15" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="L15" s="12" t="s">
+      <c r="L15" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="18" t="s">
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="34" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="37"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="19"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="35"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="19"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="35"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="37"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="20"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="36"/>
     </row>
     <row r="19" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>4</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="34" t="s">
         <v>139</v>
       </c>
       <c r="D19" s="8" t="s">
@@ -3465,8 +3465,8 @@
       <c r="A20" s="7">
         <v>5</v>
       </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="8" t="s">
         <v>159</v>
       </c>
@@ -3504,8 +3504,8 @@
       <c r="A21" s="7">
         <v>6</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="8" t="s">
         <v>160</v>
       </c>
@@ -3544,8 +3544,8 @@
         <f>SUM(A21+1)</f>
         <v>7</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
       <c r="D22" s="8" t="s">
         <v>161</v>
       </c>
@@ -3584,8 +3584,8 @@
         <f t="shared" ref="A23" si="0">SUM(A22+1)</f>
         <v>8</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
       <c r="D23" s="8" t="s">
         <v>162</v>
       </c>
@@ -3622,10 +3622,10 @@
         <f>SUM(A23+1)</f>
         <v>9</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="34" t="s">
         <v>140</v>
       </c>
       <c r="D24" s="8" t="s">
@@ -3666,8 +3666,8 @@
         <f>SUM(A24+1)</f>
         <v>10</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
       <c r="D25" s="8" t="s">
         <v>165</v>
       </c>
@@ -3706,8 +3706,8 @@
         <f t="shared" ref="A26:A28" si="1">SUM(A25+1)</f>
         <v>11</v>
       </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
       <c r="D26" s="8" t="s">
         <v>166</v>
       </c>
@@ -3744,8 +3744,8 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
       <c r="D27" s="8" t="s">
         <v>172</v>
       </c>
@@ -3782,8 +3782,8 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
       <c r="D28" s="8" t="s">
         <v>176</v>
       </c>
@@ -3819,17 +3819,18 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A4:C5"/>
-    <mergeCell ref="C19:C23"/>
-    <mergeCell ref="B19:B23"/>
-    <mergeCell ref="C24:C28"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="H15:H18"/>
+    <mergeCell ref="I15:I18"/>
+    <mergeCell ref="J15:J18"/>
+    <mergeCell ref="K15:K18"/>
+    <mergeCell ref="L15:L18"/>
+    <mergeCell ref="M15:M18"/>
+    <mergeCell ref="L9:L13"/>
+    <mergeCell ref="M9:M13"/>
+    <mergeCell ref="N9:N13"/>
+    <mergeCell ref="O9:O13"/>
+    <mergeCell ref="N15:N18"/>
+    <mergeCell ref="O15:O18"/>
     <mergeCell ref="J9:J13"/>
     <mergeCell ref="K9:K13"/>
     <mergeCell ref="A9:A13"/>
@@ -3846,18 +3847,17 @@
     <mergeCell ref="D15:D18"/>
     <mergeCell ref="E15:E18"/>
     <mergeCell ref="F15:F18"/>
-    <mergeCell ref="M15:M18"/>
-    <mergeCell ref="L9:L13"/>
-    <mergeCell ref="M9:M13"/>
-    <mergeCell ref="N9:N13"/>
-    <mergeCell ref="O9:O13"/>
-    <mergeCell ref="N15:N18"/>
-    <mergeCell ref="O15:O18"/>
-    <mergeCell ref="H15:H18"/>
-    <mergeCell ref="I15:I18"/>
-    <mergeCell ref="J15:J18"/>
-    <mergeCell ref="K15:K18"/>
-    <mergeCell ref="L15:L18"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A4:C5"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="C24:C28"/>
+    <mergeCell ref="B24:B28"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="G19:I28">
@@ -3961,16 +3961,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="33" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="35"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -3982,16 +3982,16 @@
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="36">
+      <c r="B2" s="19"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="27">
         <v>46113</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="43"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="38"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -4003,16 +4003,16 @@
       <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="40"/>
-      <c r="F3" s="41"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -4024,11 +4024,11 @@
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="23"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
@@ -4049,9 +4049,9 @@
       <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
       <c r="D5" s="11">
         <v>0</v>
       </c>

</xml_diff>